<commit_message>
fix IP for auto select ramp block
</commit_message>
<xml_diff>
--- a/results_tree.xlsx
+++ b/results_tree.xlsx
@@ -35,7 +35,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="000000FF"/>
+        <fgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -45,12 +45,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFF00"/>
+        <fgColor rgb="000000FF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
+        <fgColor rgb="00FFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -82,34 +82,34 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:AH7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,6 +496,28 @@
     <col width="8" customWidth="1" min="9" max="9"/>
     <col width="8" customWidth="1" min="10" max="10"/>
     <col width="8" customWidth="1" min="11" max="11"/>
+    <col width="8" customWidth="1" min="12" max="12"/>
+    <col width="8" customWidth="1" min="13" max="13"/>
+    <col width="8" customWidth="1" min="14" max="14"/>
+    <col width="8" customWidth="1" min="15" max="15"/>
+    <col width="8" customWidth="1" min="16" max="16"/>
+    <col width="8" customWidth="1" min="17" max="17"/>
+    <col width="8" customWidth="1" min="18" max="18"/>
+    <col width="8" customWidth="1" min="19" max="19"/>
+    <col width="8" customWidth="1" min="20" max="20"/>
+    <col width="8" customWidth="1" min="21" max="21"/>
+    <col width="8" customWidth="1" min="22" max="22"/>
+    <col width="8" customWidth="1" min="23" max="23"/>
+    <col width="8" customWidth="1" min="24" max="24"/>
+    <col width="8" customWidth="1" min="25" max="25"/>
+    <col width="8" customWidth="1" min="26" max="26"/>
+    <col width="8" customWidth="1" min="27" max="27"/>
+    <col width="8" customWidth="1" min="28" max="28"/>
+    <col width="8" customWidth="1" min="29" max="29"/>
+    <col width="8" customWidth="1" min="30" max="30"/>
+    <col width="8" customWidth="1" min="31" max="31"/>
+    <col width="8" customWidth="1" min="32" max="32"/>
+    <col width="8" customWidth="1" min="33" max="33"/>
   </cols>
   <sheetData>
     <row r="1" ht="32" customHeight="1">
@@ -504,46 +526,145 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
+          <t>←
+→</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>←
+→</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>←
+→</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>←
+→</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>←
+→</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>←
+→</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="N1" s="2" t="inlineStr">
+        <is>
+          <t>←
+→</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="P1" s="2" t="inlineStr">
+        <is>
+          <t>←
+→</t>
+        </is>
+      </c>
+      <c r="Q1" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="R1" s="2" t="inlineStr">
+        <is>
           <t>→
 ←</t>
         </is>
       </c>
-      <c r="C1" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="S1" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="T1" s="2" t="inlineStr">
         <is>
           <t>→
 ←</t>
         </is>
       </c>
-      <c r="E1" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="U1" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="V1" s="2" t="inlineStr">
         <is>
           <t>→
 ←</t>
         </is>
       </c>
-      <c r="G1" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="W1" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="X1" s="2" t="inlineStr">
         <is>
           <t>→
 ←</t>
         </is>
       </c>
-      <c r="I1" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="K1" s="2" t="inlineStr">
+      <c r="Y1" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="Z1" s="2" t="inlineStr">
+        <is>
+          <t>→
+←</t>
+        </is>
+      </c>
+      <c r="AA1" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="AB1" s="2" t="inlineStr">
+        <is>
+          <t>→
+←</t>
+        </is>
+      </c>
+      <c r="AC1" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="AD1" s="2" t="inlineStr">
+        <is>
+          <t>→
+←</t>
+        </is>
+      </c>
+      <c r="AE1" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="AG1" s="2" t="inlineStr">
         <is>
           <t>car</t>
         </is>
       </c>
-      <c r="L1" s="2" t="inlineStr">
+      <c r="AH1" s="2" t="inlineStr">
         <is>
           <t>LP → DP</t>
         </is>
@@ -557,78 +678,193 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
+          <t>↓↑</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
           <t>↑</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="K2" s="5" t="inlineStr">
+          <t>↓↑</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="inlineStr">
+        <is>
+          <t>↓↑</t>
+        </is>
+      </c>
+      <c r="M2" s="2" t="inlineStr">
+        <is>
+          <t>↓↑</t>
+        </is>
+      </c>
+      <c r="O2" s="2" t="inlineStr">
+        <is>
+          <t>↓↑</t>
+        </is>
+      </c>
+      <c r="Q2" s="2" t="inlineStr">
+        <is>
+          <t>↓↑</t>
+        </is>
+      </c>
+      <c r="S2" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="U2" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="W2" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="Y2" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="AA2" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="AC2" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="AE2" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="AG2" s="5" t="inlineStr">
         <is>
           <t>car 1</t>
         </is>
       </c>
-      <c r="L2" s="2" t="inlineStr">
-        <is>
-          <t>3 → 9</t>
+      <c r="AH2" s="2" t="inlineStr">
+        <is>
+          <t>2 → 4</t>
         </is>
       </c>
     </row>
     <row r="3" ht="32" customHeight="1">
       <c r="A3" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
+        <v>16</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">→
 </t>
         </is>
       </c>
-      <c r="C3" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">→
-</t>
-        </is>
-      </c>
-      <c r="E3" s="6" t="n">
-        <v>7</v>
-      </c>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">→
-</t>
-        </is>
-      </c>
-      <c r="G3" s="3" t="n">
-        <v>8</v>
+      <c r="E3" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="G3" s="6" t="n">
+        <v>19</v>
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>→
-←</t>
-        </is>
-      </c>
-      <c r="I3" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="K3" s="7" t="inlineStr">
+          <t>←</t>
+        </is>
+      </c>
+      <c r="I3" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="K3" s="6" t="n">
+        <v>21</v>
+      </c>
+      <c r="M3" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="O3" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q3" s="7" t="n">
+        <v>24</v>
+      </c>
+      <c r="R3" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="S3" s="7" t="n">
+        <v>25</v>
+      </c>
+      <c r="T3" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="U3" s="7" t="n">
+        <v>26</v>
+      </c>
+      <c r="V3" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="W3" s="7" t="n">
+        <v>27</v>
+      </c>
+      <c r="X3" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="Y3" s="7" t="n">
+        <v>28</v>
+      </c>
+      <c r="Z3" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="AA3" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AB3" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="AC3" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AD3" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="AE3" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="AG3" s="8" t="inlineStr">
         <is>
           <t>car 2</t>
         </is>
       </c>
-      <c r="L3" s="2" t="inlineStr">
-        <is>
-          <t>2 → 6</t>
+      <c r="AH3" s="2" t="inlineStr">
+        <is>
+          <t>2 → 9</t>
         </is>
       </c>
     </row>
@@ -638,68 +874,196 @@
           <t>↓↑</t>
         </is>
       </c>
-      <c r="G4" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>↑</t>
         </is>
       </c>
       <c r="I4" s="2" t="inlineStr">
         <is>
-          <t>↓↑</t>
-        </is>
-      </c>
-      <c r="K4" s="8" t="inlineStr">
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="K4" s="2" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="M4" s="2" t="inlineStr">
+        <is>
+          <t>↓↑</t>
+        </is>
+      </c>
+      <c r="O4" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="Q4" s="2" t="inlineStr">
+        <is>
+          <t>↓↑</t>
+        </is>
+      </c>
+      <c r="W4" s="2" t="inlineStr">
+        <is>
+          <t>↓↑</t>
+        </is>
+      </c>
+      <c r="Y4" s="2" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="AA4" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="AC4" s="2" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="AE4" s="2" t="inlineStr">
+        <is>
+          <t>↓↑</t>
+        </is>
+      </c>
+      <c r="AG4" s="9" t="inlineStr">
         <is>
           <t>car 3</t>
         </is>
       </c>
-      <c r="L4" s="2" t="inlineStr">
-        <is>
-          <t>2 → 8</t>
+      <c r="AH4" s="2" t="inlineStr">
+        <is>
+          <t>8 → 9</t>
         </is>
       </c>
     </row>
     <row r="5" ht="32" customHeight="1">
       <c r="A5" s="6" t="n">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>33</v>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">→
+</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
         <is>
           <t>→
 ←</t>
         </is>
       </c>
-      <c r="C5" s="6" t="n">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
+      <c r="G5" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="H5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="I5" s="6" t="n">
+        <v>36</v>
+      </c>
+      <c r="J5" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">→
+</t>
+        </is>
+      </c>
+      <c r="K5" s="6" t="n">
+        <v>37</v>
+      </c>
+      <c r="M5" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="N5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="O5" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="Q5" s="7" t="n">
+        <v>40</v>
+      </c>
+      <c r="R5" s="2" t="inlineStr">
         <is>
           <t>→
 ←</t>
         </is>
       </c>
-      <c r="E5" s="6" t="n">
-        <v>12</v>
-      </c>
-      <c r="F5" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="G5" s="4" t="n">
-        <v>13</v>
-      </c>
-      <c r="I5" s="3" t="n">
-        <v>14</v>
-      </c>
-      <c r="K5" s="9" t="inlineStr">
+      <c r="S5" s="7" t="n">
+        <v>41</v>
+      </c>
+      <c r="T5" s="2" t="inlineStr">
+        <is>
+          <t>→
+←</t>
+        </is>
+      </c>
+      <c r="U5" s="7" t="n">
+        <v>42</v>
+      </c>
+      <c r="W5" s="7" t="n">
+        <v>43</v>
+      </c>
+      <c r="X5" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">→
+</t>
+        </is>
+      </c>
+      <c r="Y5" s="7" t="n">
+        <v>44</v>
+      </c>
+      <c r="Z5" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="AA5" s="4" t="n">
+        <v>45</v>
+      </c>
+      <c r="AB5" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">→
+</t>
+        </is>
+      </c>
+      <c r="AC5" s="4" t="n">
+        <v>46</v>
+      </c>
+      <c r="AE5" s="4" t="n">
+        <v>47</v>
+      </c>
+      <c r="AG5" s="10" t="inlineStr">
         <is>
           <t>car 4</t>
         </is>
       </c>
-      <c r="L5" s="2" t="inlineStr">
-        <is>
-          <t>5 → 7</t>
+      <c r="AH5" s="2" t="inlineStr">
+        <is>
+          <t>7 → 8</t>
         </is>
       </c>
     </row>
@@ -714,109 +1078,163 @@
           <t>↓↑</t>
         </is>
       </c>
-      <c r="G6" s="2" t="inlineStr">
-        <is>
-          <t>↓↑</t>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="I6" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="K6" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="M6" s="2" t="inlineStr">
+        <is>
+          <t>↓↑</t>
+        </is>
+      </c>
+      <c r="O6" s="2" t="inlineStr">
+        <is>
+          <t>↓↑</t>
+        </is>
+      </c>
+      <c r="Q6" s="2" t="inlineStr">
+        <is>
+          <t>↓↑</t>
+        </is>
+      </c>
+      <c r="S6" s="2" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="U6" s="2" t="inlineStr">
+        <is>
+          <t>↓↑</t>
+        </is>
+      </c>
+      <c r="W6" s="2" t="inlineStr">
+        <is>
+          <t>↓↑</t>
+        </is>
+      </c>
+      <c r="Y6" s="2" t="inlineStr">
+        <is>
+          <t>↓↑</t>
+        </is>
+      </c>
+      <c r="AA6" s="2" t="inlineStr">
+        <is>
+          <t>↓↑</t>
+        </is>
+      </c>
+      <c r="AC6" s="2" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="AE6" s="2" t="inlineStr">
+        <is>
+          <t>↓</t>
         </is>
       </c>
     </row>
     <row r="7" ht="32" customHeight="1">
-      <c r="A7" s="4" t="n">
-        <v>15</v>
-      </c>
-      <c r="C7" s="10" t="n">
-        <v>16</v>
+      <c r="A7" s="6" t="n">
+        <v>48</v>
+      </c>
+      <c r="C7" s="6" t="n">
+        <v>49</v>
       </c>
       <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">→
+</t>
+        </is>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
         <is>
           <t>→
 ←</t>
         </is>
       </c>
-      <c r="E7" s="10" t="n">
-        <v>17</v>
-      </c>
-      <c r="G7" s="4" t="n">
-        <v>18</v>
+      <c r="G7" s="6" t="n">
+        <v>51</v>
       </c>
       <c r="H7" s="2" t="inlineStr">
         <is>
-          <t>→
-←</t>
-        </is>
-      </c>
-      <c r="I7" s="4" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" ht="32" customHeight="1">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>↓↑</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="E8" s="2" t="inlineStr">
-        <is>
-          <t>↓</t>
-        </is>
-      </c>
-      <c r="G8" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-      <c r="I8" s="2" t="inlineStr">
-        <is>
-          <t>↑</t>
-        </is>
-      </c>
-    </row>
-    <row r="9" ht="32" customHeight="1">
-      <c r="A9" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="B9" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="C9" s="10" t="n">
-        <v>21</v>
-      </c>
-      <c r="D9" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="E9" s="10" t="n">
-        <v>22</v>
-      </c>
-      <c r="F9" s="2" t="inlineStr">
+          <t>←</t>
+        </is>
+      </c>
+      <c r="I7" s="6" t="n">
+        <v>52</v>
+      </c>
+      <c r="J7" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="K7" s="6" t="n">
+        <v>53</v>
+      </c>
+      <c r="M7" s="6" t="n">
+        <v>54</v>
+      </c>
+      <c r="O7" s="6" t="n">
+        <v>55</v>
+      </c>
+      <c r="Q7" s="7" t="n">
+        <v>56</v>
+      </c>
+      <c r="R7" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">→
 </t>
         </is>
       </c>
-      <c r="G9" s="10" t="n">
-        <v>23</v>
-      </c>
-      <c r="H9" s="2" t="inlineStr">
+      <c r="S7" s="7" t="n">
+        <v>57</v>
+      </c>
+      <c r="U7" s="7" t="n">
+        <v>58</v>
+      </c>
+      <c r="W7" s="7" t="n">
+        <v>59</v>
+      </c>
+      <c r="Y7" s="7" t="n">
+        <v>60</v>
+      </c>
+      <c r="AA7" s="4" t="n">
+        <v>61</v>
+      </c>
+      <c r="AB7" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">→
 </t>
         </is>
       </c>
-      <c r="I9" s="10" t="n">
-        <v>24</v>
+      <c r="AC7" s="4" t="n">
+        <v>62</v>
+      </c>
+      <c r="AD7" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="AE7" s="4" t="n">
+        <v>63</v>
       </c>
     </row>
-    <row r="10" ht="32" customHeight="1"/>
-    <row r="11" ht="32" customHeight="1"/>
+    <row r="8" ht="32" customHeight="1"/>
+    <row r="9" ht="32" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>